<commit_message>
Update api specification xlsx, remove old file
</commit_message>
<xml_diff>
--- a/api_specification.xlsx
+++ b/api_specification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27618"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domar\Desktop\FS24_repos\laser-chad-fullstack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{488DBE38-043C-4DFB-A8F8-C8381E82833A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C736110A-193A-464C-968E-F360DE4E03C8}"/>
+  <xr:revisionPtr revIDLastSave="245" documentId="13_ncr:1_{488DBE38-043C-4DFB-A8F8-C8381E82833A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2D6C478-1FCB-4C73-A8EE-F2DD90B481A6}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="2535" windowWidth="28800" windowHeight="15435" xr2:uid="{F74C8C5D-C818-4AEC-B1C1-B5E72E720C2A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="87">
   <si>
     <t>implemented?</t>
   </si>
@@ -62,7 +62,7 @@
     <t>YES</t>
   </si>
   <si>
-    <t>/product-microservice/product</t>
+    <t>/product</t>
   </si>
   <si>
     <t>GET</t>
@@ -83,7 +83,10 @@
     <t>overwrite if exists</t>
   </si>
   <si>
-    <t>/product-microservice/product/{productId}</t>
+    <t>/product/{productId}</t>
+  </si>
+  <si>
+    <t>PRODUCT NOT RETURNED (when new product created)</t>
   </si>
   <si>
     <t>Get product with productId</t>
@@ -92,7 +95,16 @@
     <t>empty if not found</t>
   </si>
   <si>
-    <t>/product-microservice/product-detail</t>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>Delete product Comment and Details with productId</t>
+  </si>
+  <si>
+    <t>Wont throw 404</t>
+  </si>
+  <si>
+    <t>/product-detail</t>
   </si>
   <si>
     <t>Get all product details</t>
@@ -101,13 +113,13 @@
     <t>Post a product detail</t>
   </si>
   <si>
-    <t>/product-microservice/product-detail/{productId}</t>
+    <t>/product-detail/{productId}</t>
   </si>
   <si>
     <t>Get product details with productId</t>
   </si>
   <si>
-    <t>/product-microservice/product-comment</t>
+    <t>/product-comment</t>
   </si>
   <si>
     <t>Get all product comments</t>
@@ -116,7 +128,20 @@
     <t>Post a product comment</t>
   </si>
   <si>
-    <t>/product-microservice/product-comment/{productId}</t>
+    <t>Posting format:
+"product_id": "2",
+    "reviews": [
+      {
+        "user": "GamerGal83",
+        "rating": 4.5,
+        "title": "Awesome for Gaming on the Go",
+        "comment": "I love the portability and the battery life is decent enough for my gaming sessions.",
+        "date": "2024-03-10"
+      }
+]</t>
+  </si>
+  <si>
+    <t>/product-comment/{productId}</t>
   </si>
   <si>
     <t>Get product comments with productId</t>
@@ -131,63 +156,78 @@
     <t>Get order with orderId</t>
   </si>
   <si>
+    <t>/order/{user_id}</t>
+  </si>
+  <si>
+    <t>Creates an order from users cart, empties users cart</t>
+  </si>
+  <si>
+    <t>return all order objects of user</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Updates Status of order</t>
+  </si>
+  <si>
+    <t>/cart/{userId}</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>the cart</t>
+  </si>
+  <si>
+    <t>Get cart with userId</t>
+  </si>
+  <si>
+    <t>404 is not userId cart</t>
+  </si>
+  <si>
+    <t>409 if conflict userId</t>
+  </si>
+  <si>
     <t>productId</t>
   </si>
   <si>
-    <t>Add productId to orderId</t>
-  </si>
-  <si>
-    <t>allow duplicates</t>
-  </si>
-  <si>
-    <t>DELETE</t>
-  </si>
-  <si>
-    <t>Delete the whole order with orderId</t>
-  </si>
-  <si>
-    <t>Delete productId from orderId</t>
-  </si>
-  <si>
-    <t>/cart/{userId}</t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t>the cart</t>
-  </si>
-  <si>
-    <t>Get cart with userId</t>
-  </si>
-  <si>
-    <t>404 is not userId cart</t>
-  </si>
-  <si>
-    <t>Create cart with userId, cart is empty</t>
-  </si>
-  <si>
-    <t>409 if conflict userId</t>
-  </si>
-  <si>
-    <t>PUT</t>
-  </si>
-  <si>
     <t>the updated cart</t>
   </si>
   <si>
-    <t>Update cart, add one qty to productId, put there if not yet exist</t>
+    <t>Update cart, add one quantity to productId, put there if not yet exist</t>
   </si>
   <si>
     <t>success if exists, cart is unchanged, 404 if userId has no cart</t>
   </si>
   <si>
-    <t>Update cart, remove one qty from product with productId</t>
+    <t>Update cart, remove one quantity from product with productId</t>
   </si>
   <si>
     <t>success if not exist, cart is unchanged, 404 if userId has no cart</t>
   </si>
   <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>/cart/{userId}/batch</t>
+  </si>
+  <si>
+    <t>products: array[] | array[{product_id:str, quantity:int}]</t>
+  </si>
+  <si>
+    <t>TODO: cart updated?</t>
+  </si>
+  <si>
+    <t>Replace prodcuts entry for userId with products from body, can be empty array</t>
+  </si>
+  <si>
+    <t>404 if not userId cart</t>
+  </si>
+  <si>
     <t>/user/{userId}</t>
   </si>
   <si>
@@ -204,13 +244,152 @@
   </si>
   <si>
     <t>Post the picture of shopId</t>
+  </si>
+  <si>
+    <t>wishes</t>
+  </si>
+  <si>
+    <t>/sales-microservice/product/{username}</t>
+  </si>
+  <si>
+    <t>all products for a specific user (all purchases / online items)</t>
+  </si>
+  <si>
+    <t>[
+  {
+    "product_id": 1,
+    "product": "Dell XPS 15",
+    "highlighted": false,
+    "images": [
+      "https://www.digitec.ch/im/Files/2/0/3/5/9/6/0/8/UBVBa-7VUE-i5Djte0yBlA.r.jpg?impolicy=ProductTileImage&amp;resizeWidth=648&amp;resizeHeight=486&amp;cropWidth=648&amp;cropHeight=486&amp;resizeType=downsize&amp;quality=high",
+      "https://www.digitec.ch/im/Files/2/0/3/5/9/6/1/0/RDBxIBAIbU6m34Onj9Vk3Q.r.jpg?impolicy=ProductTileImage&amp;resizeWidth=648&amp;resizeHeight=486&amp;cropWidth=648&amp;cropHeight=486&amp;resizeType=downsize&amp;quality=high",
+      "https://www.digitec.ch/im/Files/2/0/3/5/9/6/0/3/kcEBwORP00e9EB0fn8fu-g.r.jpg?impolicy=ProductTileImage&amp;resizeWidth=500&amp;resizeHeight=375&amp;cropWidth=500&amp;cropHeight=375&amp;resizeType=downsize&amp;quality=high",
+      "https://www.digitec.ch/im/Files/2/0/3/5/9/6/0/5/VXCQVm1wgE-HmVUOAo7giQ.r.jpg?impolicy=ProductTileImage&amp;resizeWidth=500&amp;resizeHeight=375&amp;cropWidth=500&amp;cropHeight=375&amp;resizeType=downsize&amp;quality=high",
+      "https://www.digitec.ch/im/Files/2/0/3/5/9/6/0/6/OZ3zMe835UW2qF2zH-VWxQ.r.jpg?impolicy=ProductTileImage&amp;resizeWidth=500&amp;resizeHeight=375&amp;cropWidth=500&amp;cropHeight=375&amp;resizeType=downsize&amp;quality=high"
+    ],
+    "price": 17.32,
+    "formatted_text": "",
+    "category": "Tech",
+    "brand": "Dell",
+    "subheader": "13.50\", Intel Core i5-1145G7, 8 GB, 256 GB, DE",
+    "technical_details": {
+      "processor": "Intel Core i7",
+      "ram": "16GB",
+      "storage": "512GB SSD",
+      "screen": "15.6-inch 4K UHD",
+      "battery": "86Wh",
+      "operating_system": "Windows 10 Home",
+      "graphics": "NVproduct_idIA GeForce GTX 1650 Ti",
+      "ports": {
+        "usb_c": 2,
+        "hdmi": 1,
+        "headphone_jack": 1,
+        "sd_card_reader": 1
+      },
+      "weight": "1.83kg"
+    },
+    "warranty": "1 year",
+    "color": "Silver",
+    "description": "A powerful and versatile laptop designed for performance and portability. Featuring a stunning 4K UHD display and a robust technical specification list, the Dell XPS 15 is ideal for both professional and personal use.",
+    "availability": "In stock",
+    "seller": "nicolas.meyer2@outlook.com"
+  },... more like this]</t>
+  </si>
+  <si>
+    <t>&gt; we could do several api calls for the same object but in the end it should be the same object with the same structure =&gt; if exists then list the calls pls &lt;3</t>
+  </si>
+  <si>
+    <t>Thanks!
+distributor and category are not currently available</t>
+  </si>
+  <si>
+    <t>deletes by Id (or flags as inactive or sets the stock to 0 such that it cannot be bought anymore)</t>
+  </si>
+  <si>
+    <t>/distributor</t>
+  </si>
+  <si>
+    <t>returns all distibutors from the database</t>
+  </si>
+  <si>
+    <t>[
+  {
+    "name": "TechNova",
+    "industry": "Technology",
+    "headquarters": "San Francisco, CA, USA",
+    "numberOfEmployees": 5000,
+    "foundationYear": 2001
+  },... more companies in our database...] =&gt; i just care about the name tbh. the other attributes idc about</t>
+  </si>
+  <si>
+    <t>/category</t>
+  </si>
+  <si>
+    <t>returns all categories from the database</t>
+  </si>
+  <si>
+    <t>[
+  {
+    "id": 1,
+    "name": "Tech",
+    "options": [
+      "connectivity",
+      "warranty period",
+      "brand",
+      "energy efficiency",
+      "compatibility"
+    ]
+  },... more objects with name and options]</t>
+  </si>
+  <si>
+    <t>/product-comment/{product_id}</t>
+  </si>
+  <si>
+    <t>review_id</t>
+  </si>
+  <si>
+    <t>ENHANCE</t>
+  </si>
+  <si>
+    <t>return ID for comment as well (currently missing)</t>
+  </si>
+  <si>
+    <t>review object with review_id</t>
+  </si>
+  <si>
+    <t>{
+    "product_id": "uuxpxjb9i",
+    "product": "some test",
+    "subheader": "some random subheader",
+    "warranty": "2 years",
+    "description": "some description",
+    "price": 999,
+    "category": "Laptop",
+    "brand": "EduFuture",
+    "technical_details": {
+        "some spec1": "some value 1",
+        "some spec2": "some val 2"
+    },
+    "images": [
+        "blob:http://localhost:3000/a470365f-e340-48a2-bcf9-2218c6a8fecd",
+        "blob:http://localhost:3000/9efb9be7-cc14-4f24-984a-62fc7c607a76",
+        "blob:http://localhost:3000/4dc55dcd-6350-45b3-8f06-d760d416cda2"
+    ],
+    "availability": "Not available"
+}</t>
+  </si>
+  <si>
+    <t>returns product ID when created successfullly</t>
+  </si>
+  <si>
+    <t>&gt; attention: technical details differ for every product</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,8 +411,14 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,6 +479,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -307,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -336,6 +533,33 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,8 +625,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{40BB7AFB-9880-43BB-81AD-FB2DB22BFC51}" name="Tabelle1" displayName="Tabelle1" ref="B1:G22" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="B1:G22" xr:uid="{40BB7AFB-9880-43BB-81AD-FB2DB22BFC51}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{40BB7AFB-9880-43BB-81AD-FB2DB22BFC51}" name="Tabelle1" displayName="Tabelle1" ref="B1:G24" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="B1:G24" xr:uid="{40BB7AFB-9880-43BB-81AD-FB2DB22BFC51}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{49643829-E905-4014-B0C3-4AFC6C144315}" name="path" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FFAD1BBA-D8F6-4566-9A4C-F7CAE1EF24EE}" name="method" dataDxfId="3"/>
@@ -732,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9389E75-8D37-4FF0-A463-5929B09551A5}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="19.5" customHeight="1"/>
@@ -743,7 +967,7 @@
     <col min="2" max="2" width="45.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="98.28515625" customWidth="1"/>
     <col min="6" max="6" width="59.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="56.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -808,83 +1032,85 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1" t="s">
+      <c r="D4" s="20"/>
+      <c r="E4" s="20" t="s">
         <v>16</v>
       </c>
+      <c r="F4" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="G4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="19.5" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="19.5" customHeight="1">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="19.5" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A8" s="8"/>
+      <c r="A8" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>9</v>
@@ -892,154 +1118,154 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="19.5" customHeight="1">
       <c r="A9" s="8"/>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="19.5" customHeight="1">
       <c r="A10" s="8"/>
-      <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A11" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="A11" s="8"/>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>17</v>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="19.5" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="C12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="19.5" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="19.5" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A15" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="7" t="s">
+      <c r="A15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="D15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="19.5" customHeight="1">
       <c r="A16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="C16" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="E16" s="7" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="19.5" customHeight="1">
@@ -1048,16 +1274,14 @@
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>46</v>
+      <c r="F17" s="7">
+        <v>1</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>47</v>
@@ -1069,94 +1293,271 @@
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="7" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A19" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="F19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A20" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A21" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A20" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6" t="s">
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A22" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" s="6" t="s">
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A21" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="13" t="s">
+    <row r="23" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A23" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13" t="s">
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A24" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="19.5" customHeight="1">
+      <c r="B36" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A37" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F37" s="18"/>
+    </row>
+    <row r="38" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A38" s="23"/>
+      <c r="B38" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="87" customHeight="1">
+      <c r="A39" s="23"/>
+      <c r="B39" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A40" t="s">
         <v>54</v>
       </c>
-      <c r="G21" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A22" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13" t="s">
+      <c r="B40" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="19.5" customHeight="1">
+      <c r="B42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>14</v>
+      <c r="D42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A45" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G45" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A37:A39"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -1175,16 +1576,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2109d437-7f39-46d1-b177-edfd83cf9b84">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AD2C30D497D667408D1ABF0DAAD9346F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b97394f073c24990fb0fda386d171f3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2109d437-7f39-46d1-b177-edfd83cf9b84" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5a2b2b98103c7d23f0c8d453555bf1f2" ns2:_="">
     <xsd:import namespace="2109d437-7f39-46d1-b177-edfd83cf9b84"/>
@@ -1368,14 +1759,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2109d437-7f39-46d1-b177-edfd83cf9b84">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{655A35DF-7D10-48B6-A29D-7F386BB24094}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1F5D4E7-92AC-4EAB-B68F-A242664F8446}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C52283C9-82EF-4633-A0F1-B7D2387E8C8B}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C52283C9-82EF-4633-A0F1-B7D2387E8C8B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1F5D4E7-92AC-4EAB-B68F-A242664F8446}"/>
 </file>
</xml_diff>